<commit_message>
Gen 7, volat corrected, new TSS
</commit_message>
<xml_diff>
--- a/DataInput/Tables/DataSource/SoilCharacteristics_Alteck.xlsx
+++ b/DataInput/Tables/DataSource/SoilCharacteristics_Alteck.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DayTightChunks/Documents/PhD/Models/phd-model-master/DataInput/Tables/DataSource/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14715" yWindow="0" windowWidth="10485" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="8780" yWindow="460" windowWidth="16420" windowHeight="13860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wcm" sheetId="1" r:id="rId1"/>
@@ -15,9 +20,18 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">p_b!$A$1:$C$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Wcm!$A$1:$A$95</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -80,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="56">
   <si>
     <t>W100</t>
   </si>
@@ -242,6 +256,12 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Mean &lt; 30cm</t>
+  </si>
+  <si>
+    <t>SD &lt; 30cm</t>
   </si>
 </sst>
 </file>
@@ -808,7 +828,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -850,12 +870,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -885,12 +905,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1100,12 +1120,12 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="2" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -1122,7 +1142,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1160,7 @@
         <v>0.39854204114240033</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1158,7 +1178,7 @@
         <v>0.39794287996804467</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +1196,7 @@
         <v>0.39444777311763529</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1214,7 @@
         <v>0.37147992810065894</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1232,7 @@
         <v>0.39245056920311577</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1230,7 +1250,7 @@
         <v>0.38635909726383061</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1268,7 @@
         <v>0.39285000998601932</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1266,7 +1286,7 @@
         <v>0.36668663870581159</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +1304,7 @@
         <v>0.37437587377671266</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1322,7 @@
         <v>0.36089474735370469</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +1340,7 @@
         <v>0.35869782304773334</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1338,7 +1358,7 @@
         <v>0.35879768324345868</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1356,7 +1376,7 @@
         <v>0.34381865388456112</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1374,7 +1394,7 @@
         <v>0.34291991212302753</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1412,7 @@
         <v>0.32794088276412997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1410,7 +1430,7 @@
         <v>0.41961254244058299</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1428,7 +1448,7 @@
         <v>0.42480527261833395</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1446,7 +1466,7 @@
         <v>0.43039744357898907</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1464,7 +1484,7 @@
         <v>0.40213700818853587</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1482,7 +1502,7 @@
         <v>0.40183742760135821</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1500,7 +1520,7 @@
         <v>0.41242260834831246</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1518,7 +1538,7 @@
         <v>0.34252047134012392</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1536,7 +1556,7 @@
         <v>0.34172158977431621</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1554,7 +1574,7 @@
         <v>0.33922508488116609</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +1592,7 @@
         <v>0.36079488715797881</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1590,7 +1610,7 @@
         <v>0.37217894947074076</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1608,7 +1628,7 @@
         <v>0.37157978829638483</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1626,7 +1646,7 @@
         <v>0.37767126023567055</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1644,7 +1664,7 @@
         <v>0.40343519073297363</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1662,7 +1682,7 @@
         <v>0.41661673656880338</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1680,7 +1700,7 @@
         <v>0.31625723986419002</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1698,7 +1718,7 @@
         <v>0.32474535650089886</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1716,7 +1736,7 @@
         <v>0.33263431196325116</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1734,7 +1754,7 @@
         <v>0.35560215698022779</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1752,7 +1772,7 @@
         <v>0.37048132614339918</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1770,7 +1790,7 @@
         <v>0.38546035550229646</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -1788,7 +1808,7 @@
         <v>0.40922708208508052</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1806,7 +1826,7 @@
         <v>0.40383463151587773</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1824,7 +1844,7 @@
         <v>0.39205112842021161</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -1842,7 +1862,7 @@
         <v>0.36808468144597578</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +1880,7 @@
         <v>0.37108048731775484</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1878,7 +1898,7 @@
         <v>0.36858398242460583</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -1896,7 +1916,7 @@
         <v>0.368284401837427</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -1914,7 +1934,7 @@
         <v>0.38785700019972069</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -1932,7 +1952,7 @@
         <v>0.49440782903934483</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -1950,7 +1970,7 @@
         <v>0.35370481326143388</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1968,7 +1988,7 @@
         <v>0.36978230477331736</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -1986,7 +2006,7 @@
         <v>0.37287797084082286</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2004,7 +2024,7 @@
         <v>0.32903934491711589</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -2022,7 +2042,7 @@
         <v>0.33233473137607322</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -2040,7 +2060,7 @@
         <v>0.32923906530856828</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2078,7 @@
         <v>0.36488915518274379</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -2076,7 +2096,7 @@
         <v>0.36249251048532066</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -2094,7 +2114,7 @@
         <v>0.37257839025364464</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -2112,7 +2132,7 @@
         <v>0.3634911124425807</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -2130,7 +2150,7 @@
         <v>0.35799880167765152</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -2148,7 +2168,7 @@
         <v>0.36888356301178349</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -2166,7 +2186,7 @@
         <v>0.37407629318953445</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -2184,7 +2204,7 @@
         <v>0.4023367285799882</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>30</v>
       </c>
@@ -2202,7 +2222,7 @@
         <v>0.38376273217495482</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -2220,7 +2240,7 @@
         <v>0.37807070101857354</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -2238,7 +2258,7 @@
         <v>0.39265028959456783</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -2256,7 +2276,7 @@
         <v>0.3873576992210907</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -2274,7 +2294,7 @@
         <v>0.36339125224685426</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -2292,7 +2312,7 @@
         <v>0.33832634311963244</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>30</v>
       </c>
@@ -2310,7 +2330,7 @@
         <v>0.35010984621529834</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -2328,7 +2348,7 @@
         <v>0.35700019972039143</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>29</v>
       </c>
@@ -2346,7 +2366,7 @@
         <v>0.35370481326143416</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>30</v>
       </c>
@@ -2364,7 +2384,7 @@
         <v>0.35260635110844818</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -2382,7 +2402,7 @@
         <v>0.3665867785100857</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -2400,7 +2420,7 @@
         <v>0.35110844817255865</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>30</v>
       </c>
@@ -2418,7 +2438,7 @@
         <v>0.35620131815458372</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -2436,7 +2456,7 @@
         <v>0.3802676253245455</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -2454,7 +2474,7 @@
         <v>0.37397643299380856</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>0.37577391651687575</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -2490,7 +2510,7 @@
         <v>0.38216496904333941</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -2508,7 +2528,7 @@
         <v>0.36788496105452401</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -2526,7 +2546,7 @@
         <v>0.34262033153584981</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>34</v>
       </c>
@@ -2544,7 +2564,7 @@
         <v>0.32184941082484542</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>35</v>
       </c>
@@ -2562,7 +2582,7 @@
         <v>0.32035150788895589</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -2580,7 +2600,7 @@
         <v>0.31955262632314729</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>34</v>
       </c>
@@ -2598,7 +2618,7 @@
         <v>0.37038146594767302</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>35</v>
       </c>
@@ -2616,7 +2636,7 @@
         <v>0.36908328340323582</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -2634,7 +2654,7 @@
         <v>0.38585979628520056</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -2652,7 +2672,7 @@
         <v>0.36921056819990439</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>35</v>
       </c>
@@ -2670,7 +2690,7 @@
         <v>0.38325640617539414</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>36</v>
       </c>
@@ -2688,7 +2708,7 @@
         <v>0.37736749960210103</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>34</v>
       </c>
@@ -2706,7 +2726,7 @@
         <v>0.40113840623127639</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>35</v>
       </c>
@@ -2724,7 +2744,7 @@
         <v>0.40093868583982456</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -2750,15 +2770,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C91"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2769,7 +2790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2780,7 +2801,7 @@
         <v>1.4136209306970242</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2791,7 +2812,7 @@
         <v>1.2612342720191734</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -2802,7 +2823,7 @@
         <v>1.5414419812262834</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2812,8 +2833,14 @@
       <c r="C5">
         <v>1.4958058717795089</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2823,8 +2850,16 @@
       <c r="C6">
         <v>1.5210705012981824</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>AVERAGE(C5:C91)</f>
+        <v>1.4967433697378743</v>
+      </c>
+      <c r="F6">
+        <f>STDEVA(C5:C91)</f>
+        <v>8.720124824385507E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2835,7 +2870,7 @@
         <v>1.5271619732374675</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2846,7 +2881,7 @@
         <v>1.5047932893948472</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2857,7 +2892,7 @@
         <v>1.5229678450169764</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2868,7 +2903,7 @@
         <v>1.5437387657279809</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -2879,7 +2914,7 @@
         <v>1.5917715198721794</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2890,7 +2925,7 @@
         <v>1.5621130417415616</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2901,7 +2936,7 @@
         <v>1.5630117835030957</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2912,7 +2947,7 @@
         <v>1.6672658278410228</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2923,7 +2958,7 @@
         <v>1.6693628919512684</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2934,7 +2969,7 @@
         <v>1.5462352706211306</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2945,7 +2980,7 @@
         <v>1.4854204114240064</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2956,7 +2991,7 @@
         <v>1.4751348112642304</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2967,7 +3002,7 @@
         <v>1.4383862592370682</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2978,7 +3013,7 @@
         <v>1.5148791691631713</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -2989,7 +3024,7 @@
         <v>1.4593569003395246</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -3000,7 +3035,7 @@
         <v>1.4798282404633514</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -3011,7 +3046,7 @@
         <v>1.6009586578789694</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -3022,7 +3057,7 @@
         <v>1.6293189534651484</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -3033,7 +3068,7 @@
         <v>1.5731975234671463</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -3044,7 +3079,7 @@
         <v>1.5171759536648692</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3055,7 +3090,7 @@
         <v>1.4796285200718993</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -3066,7 +3101,7 @@
         <v>1.444877171959257</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -3077,7 +3112,7 @@
         <v>1.2827042141002596</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -3088,7 +3123,7 @@
         <v>1.3055721989215099</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -3099,7 +3134,7 @@
         <v>1.3818653884561614</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -3110,7 +3145,7 @@
         <v>1.433193529059317</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -3121,7 +3156,7 @@
         <v>1.4920111843419213</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -3132,7 +3167,7 @@
         <v>1.4900139804274017</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -3143,7 +3178,7 @@
         <v>1.5240663071699621</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -3154,7 +3189,7 @@
         <v>1.4727381665668065</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -3165,7 +3200,7 @@
         <v>1.4827241861394049</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3176,7 +3211,7 @@
         <v>1.4955062911923307</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -3187,7 +3222,7 @@
         <v>1.488416217295786</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -3198,7 +3233,7 @@
         <v>1.5016976233273416</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -3209,7 +3244,7 @@
         <v>1.5929698422208909</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -3220,7 +3255,7 @@
         <v>1.5799880167765132</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -3231,7 +3266,7 @@
         <v>1.5786898342320748</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -3242,7 +3277,7 @@
         <v>1.2947872977831039</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -3253,7 +3288,7 @@
         <v>1.3246454963051726</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -3264,7 +3299,7 @@
         <v>1.2526462951867385</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -3275,7 +3310,7 @@
         <v>1.5019972039145197</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3286,7 +3321,7 @@
         <v>1.5162772119033354</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3297,7 +3332,7 @@
         <v>1.537946874375874</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3308,7 +3343,7 @@
         <v>1.5289594567605354</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -3319,7 +3354,7 @@
         <v>1.6405032953864593</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3330,7 +3365,7 @@
         <v>1.6425004993009782</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -3341,7 +3376,7 @@
         <v>1.5468344317954867</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -3352,7 +3387,7 @@
         <v>1.5496305172758136</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -3363,7 +3398,7 @@
         <v>1.5767924905132815</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -3374,7 +3409,7 @@
         <v>1.650988615937687</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -3385,7 +3420,7 @@
         <v>1.6416017575394446</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -3396,7 +3431,7 @@
         <v>1.6038546035550232</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -3407,7 +3442,7 @@
         <v>1.3980427401637707</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -3418,7 +3453,7 @@
         <v>1.4647493509087279</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -3429,7 +3464,7 @@
         <v>1.41521869382864</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -3440,7 +3475,7 @@
         <v>1.4866187337727181</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -3451,7 +3486,7 @@
         <v>1.5425404433792691</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>49</v>
       </c>
@@ -3462,7 +3497,7 @@
         <v>1.5829838226482922</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -3473,7 +3508,7 @@
         <v>1.5151787497503497</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -3484,7 +3519,7 @@
         <v>1.5329538645895744</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -3495,7 +3530,7 @@
         <v>1.5039944078290395</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -3506,7 +3541,7 @@
         <v>1.5402436588775712</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>49</v>
       </c>
@@ -3517,7 +3552,7 @@
         <v>1.5535250649091275</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -3528,7 +3563,7 @@
         <v>1.517974835230677</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>49</v>
       </c>
@@ -3539,7 +3574,7 @@
         <v>1.5358498102656282</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>49</v>
       </c>
@@ -3550,7 +3585,7 @@
         <v>1.5396444977032153</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>49</v>
       </c>
@@ -3561,7 +3596,7 @@
         <v>1.566706610744957</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>49</v>
       </c>
@@ -3572,7 +3607,7 @@
         <v>1.4195126822448572</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -3583,7 +3618,7 @@
         <v>1.4434791292190932</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>49</v>
       </c>
@@ -3594,7 +3629,7 @@
         <v>1.4425803874575598</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>50</v>
       </c>
@@ -3605,7 +3640,7 @@
         <v>1.3437187936888357</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>50</v>
       </c>
@@ -3616,7 +3651,7 @@
         <v>1.3451168364289994</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>50</v>
       </c>
@@ -3627,7 +3662,7 @@
         <v>1.3019772318753744</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>50</v>
       </c>
@@ -3638,7 +3673,7 @@
         <v>1.4780307569402835</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>50</v>
       </c>
@@ -3649,7 +3684,7 @@
         <v>1.4599560615138805</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>50</v>
       </c>
@@ -3660,7 +3695,7 @@
         <v>1.45126822448572</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>50</v>
       </c>
@@ -3671,7 +3706,7 @@
         <v>1.4556321150389455</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>50</v>
       </c>
@@ -3682,7 +3717,7 @@
         <v>1.4258038745755939</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>50</v>
       </c>
@@ -3693,7 +3728,7 @@
         <v>1.480826842420611</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>50</v>
       </c>
@@ -3704,7 +3739,7 @@
         <v>1.4746936176985517</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>50</v>
       </c>
@@ -3715,7 +3750,7 @@
         <v>1.4755689957026901</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>50</v>
       </c>
@@ -3726,7 +3761,7 @@
         <v>1.4552761419703963</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>50</v>
       </c>
@@ -3737,7 +3772,7 @@
         <v>1.4506690633113639</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>50</v>
       </c>
@@ -3748,7 +3783,7 @@
         <v>1.4525664070301576</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>50</v>
       </c>
@@ -3760,6 +3795,31 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C91">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="105-110"/>
+        <filter val="107-112"/>
+        <filter val="115-120"/>
+        <filter val="120-125"/>
+        <filter val="134-139"/>
+        <filter val="135-140"/>
+        <filter val="145-150"/>
+        <filter val="155-160*"/>
+        <filter val="165-170"/>
+        <filter val="35-40"/>
+        <filter val="40-45"/>
+        <filter val="41-46"/>
+        <filter val="45-50"/>
+        <filter val="50-55"/>
+        <filter val="65-70"/>
+        <filter val="70-75"/>
+        <filter val="75-80"/>
+        <filter val="80-85"/>
+        <filter val="95-100"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3770,7 +3830,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>